<commit_message>
Added formatting of the final page
- Sets the timeline to be the full height of the page
- Creates an index showing each category
- Sets position of each element
- Flips back and forth between each side the text goes onto
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Year</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Agriculture</t>
   </si>
   <si>
-    <t>7500 BC</t>
-  </si>
-  <si>
     <t>Wheat Cultivation Begins</t>
   </si>
   <si>
@@ -45,21 +42,12 @@
     <t>Georgraphic</t>
   </si>
   <si>
-    <t>7000 BC</t>
-  </si>
-  <si>
     <t>Neolithic Subpluvial in North Africa</t>
   </si>
   <si>
-    <t>7900 BC</t>
-  </si>
-  <si>
     <t>Civillization</t>
   </si>
   <si>
-    <t>8000 BC</t>
-  </si>
-  <si>
     <t>Urban settlement founded in Anatolia.</t>
   </si>
   <si>
@@ -81,9 +69,6 @@
     <t>The Sahara desert region supports a savanna-like environment. Lake Chad is larger than the current Caspian Sea.</t>
   </si>
   <si>
-    <t>6200 BC</t>
-  </si>
-  <si>
     <t>8.2 Kiloyear Event</t>
   </si>
   <si>
@@ -93,18 +78,12 @@
     <t>Technology</t>
   </si>
   <si>
-    <t>5500 BC</t>
-  </si>
-  <si>
     <t>Copper smelting</t>
   </si>
   <si>
     <t>Copper smelting in evidence in Plocnik and other locations.</t>
   </si>
   <si>
-    <t>5000 BC</t>
-  </si>
-  <si>
     <t>Late neolithic civillization</t>
   </si>
   <si>
@@ -112,9 +91,6 @@
   </si>
   <si>
     <t>Fertile Crescent civillization</t>
-  </si>
-  <si>
-    <t>4000 BC</t>
   </si>
   <si>
     <t>Earliest supposed dates for the domestication of the horse and for the domestication of the chicken.</t>
@@ -461,7 +437,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -486,129 +462,129 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>13</v>
+      <c r="A2">
+        <v>-8000</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>-7900</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>-7500</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>-7500</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6">
+        <v>-7000</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>-6200</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>-5500</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>-5000</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>-4000</v>
+      </c>
+      <c r="B10" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" t="s">
-        <v>31</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>